<commit_message>
added data for dfs
</commit_message>
<xml_diff>
--- a/ExperimentFiles/Experiment Results.xlsx
+++ b/ExperimentFiles/Experiment Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ituniversity-my.sharepoint.com/personal/pekd_itu_dk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andba\ITU\ResearchProject\marcusModel\swarmrobotdecisions\ExperimentFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{894ED04D-2B9A-4BED-982F-8DDF3D469760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E00BCCA8-20A3-4FC7-A183-9C59C5D35CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{ED70D03D-99F9-4705-ABBF-77F0A45A2A48}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{ED70D03D-99F9-4705-ABBF-77F0A45A2A48}"/>
   </bookViews>
   <sheets>
     <sheet name="Chart1" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="13">
   <si>
     <t>Cycles</t>
   </si>
@@ -68,12 +68,21 @@
   <si>
     <t>199/200</t>
   </si>
+  <si>
+    <t>Results for dfs-variant</t>
+  </si>
+  <si>
+    <t>Cycles dfs</t>
+  </si>
+  <si>
+    <t>(+-) dfs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +100,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,10 +138,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -146,7 +165,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="da-DK"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -317,94 +336,94 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>18.67</c:v>
+                    <c:v>18,67</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>19.5</c:v>
+                    <c:v>19,5</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>23.67</c:v>
+                    <c:v>23,67</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>23.04</c:v>
+                    <c:v>23,04</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>25.59</c:v>
+                    <c:v>25,59</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>24.64</c:v>
+                    <c:v>24,64</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>24.3</c:v>
+                    <c:v>24,3</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>29.39</c:v>
+                    <c:v>29,39</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>28.48</c:v>
+                    <c:v>28,48</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>28.5</c:v>
+                    <c:v>28,5</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>26.24</c:v>
+                    <c:v>26,24</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>30.59</c:v>
+                    <c:v>30,59</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>28.49</c:v>
+                    <c:v>28,49</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>28.14</c:v>
+                    <c:v>28,14</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>26.42</c:v>
+                    <c:v>26,42</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>25.44</c:v>
+                    <c:v>25,44</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>27.73</c:v>
+                    <c:v>27,73</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>29.07</c:v>
+                    <c:v>29,07</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>26.09</c:v>
+                    <c:v>26,09</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>24.05</c:v>
+                    <c:v>24,05</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>28.4</c:v>
+                    <c:v>28,4</c:v>
                   </c:pt>
                   <c:pt idx="21">
-                    <c:v>27.16</c:v>
+                    <c:v>27,16</c:v>
                   </c:pt>
                   <c:pt idx="22">
-                    <c:v>29.91</c:v>
+                    <c:v>29,91</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>28.49</c:v>
+                    <c:v>28,49</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>30.29</c:v>
+                    <c:v>30,29</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>31.32</c:v>
+                    <c:v>31,32</c:v>
                   </c:pt>
                   <c:pt idx="26">
-                    <c:v>28.82</c:v>
+                    <c:v>28,82</c:v>
                   </c:pt>
                   <c:pt idx="27">
-                    <c:v>30.28</c:v>
+                    <c:v>30,28</c:v>
                   </c:pt>
                   <c:pt idx="28">
-                    <c:v>31.18</c:v>
+                    <c:v>31,18</c:v>
                   </c:pt>
                   <c:pt idx="29">
-                    <c:v>30.04</c:v>
+                    <c:v>30,04</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -730,94 +749,94 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>18.67</c:v>
+                    <c:v>18,67</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>19.5</c:v>
+                    <c:v>19,5</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>23.67</c:v>
+                    <c:v>23,67</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>23.04</c:v>
+                    <c:v>23,04</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>25.59</c:v>
+                    <c:v>25,59</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>24.64</c:v>
+                    <c:v>24,64</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>24.3</c:v>
+                    <c:v>24,3</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>29.39</c:v>
+                    <c:v>29,39</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>28.48</c:v>
+                    <c:v>28,48</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>28.5</c:v>
+                    <c:v>28,5</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>26.24</c:v>
+                    <c:v>26,24</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>30.59</c:v>
+                    <c:v>30,59</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>28.49</c:v>
+                    <c:v>28,49</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>28.14</c:v>
+                    <c:v>28,14</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>26.42</c:v>
+                    <c:v>26,42</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>25.44</c:v>
+                    <c:v>25,44</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>27.73</c:v>
+                    <c:v>27,73</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>29.07</c:v>
+                    <c:v>29,07</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>26.09</c:v>
+                    <c:v>26,09</c:v>
                   </c:pt>
                   <c:pt idx="19">
-                    <c:v>24.05</c:v>
+                    <c:v>24,05</c:v>
                   </c:pt>
                   <c:pt idx="20">
-                    <c:v>28.4</c:v>
+                    <c:v>28,4</c:v>
                   </c:pt>
                   <c:pt idx="21">
-                    <c:v>27.16</c:v>
+                    <c:v>27,16</c:v>
                   </c:pt>
                   <c:pt idx="22">
-                    <c:v>29.91</c:v>
+                    <c:v>29,91</c:v>
                   </c:pt>
                   <c:pt idx="23">
-                    <c:v>28.49</c:v>
+                    <c:v>28,49</c:v>
                   </c:pt>
                   <c:pt idx="24">
-                    <c:v>30.29</c:v>
+                    <c:v>30,29</c:v>
                   </c:pt>
                   <c:pt idx="25">
-                    <c:v>31.32</c:v>
+                    <c:v>31,32</c:v>
                   </c:pt>
                   <c:pt idx="26">
-                    <c:v>28.82</c:v>
+                    <c:v>28,82</c:v>
                   </c:pt>
                   <c:pt idx="27">
-                    <c:v>30.28</c:v>
+                    <c:v>30,28</c:v>
                   </c:pt>
                   <c:pt idx="28">
-                    <c:v>31.18</c:v>
+                    <c:v>31,18</c:v>
                   </c:pt>
                   <c:pt idx="29">
-                    <c:v>30.04</c:v>
+                    <c:v>30,04</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -1805,12 +1824,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2126,22 +2141,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85E216E-DBA0-4F15-A930-31E5A6FAEE20}">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="15" max="15" width="9.85546875" customWidth="1"/>
+    <col min="15" max="15" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -2189,7 +2204,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>10</v>
       </c>
@@ -2236,7 +2251,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>20</v>
       </c>
@@ -2283,7 +2298,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>30</v>
       </c>
@@ -2330,7 +2345,7 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>40</v>
       </c>
@@ -2377,7 +2392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>50</v>
       </c>
@@ -2424,7 +2439,7 @@
         <v>2.27</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>60</v>
       </c>
@@ -2471,7 +2486,7 @@
         <v>1.57</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>70</v>
       </c>
@@ -2518,7 +2533,7 @@
         <v>2.06</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>80</v>
       </c>
@@ -2565,7 +2580,7 @@
         <v>3.34</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>90</v>
       </c>
@@ -2612,7 +2627,7 @@
         <v>2.4700000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>100</v>
       </c>
@@ -2659,7 +2674,7 @@
         <v>2.66</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>110</v>
       </c>
@@ -2706,7 +2721,7 @@
         <v>1.99</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>120</v>
       </c>
@@ -2753,7 +2768,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>130</v>
       </c>
@@ -2800,7 +2815,7 @@
         <v>3.85</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>140</v>
       </c>
@@ -2847,7 +2862,7 @@
         <v>8.69</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>150</v>
       </c>
@@ -2894,7 +2909,7 @@
         <v>6.42</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>160</v>
       </c>
@@ -2926,7 +2941,7 @@
         <v>3.24</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>170</v>
       </c>
@@ -2958,7 +2973,7 @@
         <v>5.82</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>180</v>
       </c>
@@ -2990,7 +3005,7 @@
         <v>4.71</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>190</v>
       </c>
@@ -3022,7 +3037,7 @@
         <v>8.52</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>200</v>
       </c>
@@ -3054,7 +3069,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>210</v>
       </c>
@@ -3086,7 +3101,7 @@
         <v>15.13</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>220</v>
       </c>
@@ -3103,7 +3118,7 @@
         <v>3.81</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>230</v>
       </c>
@@ -3120,7 +3135,7 @@
         <v>4.08</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>240</v>
       </c>
@@ -3137,7 +3152,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>250</v>
       </c>
@@ -3154,7 +3169,7 @@
         <v>4.7300000000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>260</v>
       </c>
@@ -3171,7 +3186,7 @@
         <v>4.54</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>270</v>
       </c>
@@ -3188,7 +3203,7 @@
         <v>4.6500000000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>280</v>
       </c>
@@ -3205,7 +3220,7 @@
         <v>4.68</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>290</v>
       </c>
@@ -3222,7 +3237,7 @@
         <v>4.91</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>300</v>
       </c>
@@ -3238,6 +3253,259 @@
       <c r="E31">
         <v>3.86</v>
       </c>
+    </row>
+    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A34" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>5.71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36">
+        <v>30000</v>
+      </c>
+      <c r="E36">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>10</v>
+      </c>
+      <c r="B37">
+        <v>6.45</v>
+      </c>
+      <c r="C37" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>30000</v>
+      </c>
+      <c r="E37">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>15</v>
+      </c>
+      <c r="B38">
+        <v>8.82</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>30000</v>
+      </c>
+      <c r="E38">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>20</v>
+      </c>
+      <c r="B39">
+        <v>14.24</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39">
+        <v>30000</v>
+      </c>
+      <c r="E39">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>25</v>
+      </c>
+      <c r="B40">
+        <v>12.67</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D40">
+        <v>30000</v>
+      </c>
+      <c r="E40">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>30</v>
+      </c>
+      <c r="B41">
+        <v>28.58</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3</v>
+      </c>
+      <c r="D41">
+        <v>30000</v>
+      </c>
+      <c r="E41">
+        <v>6.69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>35</v>
+      </c>
+      <c r="B42">
+        <v>45.29</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>30000</v>
+      </c>
+      <c r="E42">
+        <v>10.63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <v>36.11</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>30000</v>
+      </c>
+      <c r="E43">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>45</v>
+      </c>
+      <c r="B44">
+        <v>36.31</v>
+      </c>
+      <c r="C44" t="s">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>30000</v>
+      </c>
+      <c r="E44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>50</v>
+      </c>
+      <c r="B45">
+        <v>25.67</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>30000</v>
+      </c>
+      <c r="E45">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="4">
+        <v>60</v>
+      </c>
+      <c r="B46" s="4">
+        <v>20.76</v>
+      </c>
+      <c r="C46" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="5">
+        <v>30000</v>
+      </c>
+      <c r="E46" s="4">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="4">
+        <v>70</v>
+      </c>
+      <c r="B47" s="4">
+        <v>35.049999999999997</v>
+      </c>
+      <c r="C47" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>30000</v>
+      </c>
+      <c r="E47" s="4">
+        <v>6.23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="4">
+        <v>80</v>
+      </c>
+      <c r="B48" s="4">
+        <v>22.62</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>30000</v>
+      </c>
+      <c r="E48" s="4">
+        <v>2.23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="4"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>